<commit_message>
Sales Factor Weight Changes
Some changes made during the search for all of the policy implementation dates.
</commit_message>
<xml_diff>
--- a/CrossPartial/Average_SF_Weight_By_Region.xlsx
+++ b/CrossPartial/Average_SF_Weight_By_Region.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/Documents/GitHub/ST-Apportionment/CrossPartial/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E7E1BE1-BD44-A547-8316-7CE53BB1D679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D170BFB0-C7C3-B04E-BB09-46468B1AA43C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30400" yWindow="-3100" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25900" yWindow="-1300" windowWidth="19600" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Long_Gir_My_App_Comb_clean" sheetId="1" r:id="rId1"/>
@@ -751,9 +751,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -791,7 +791,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -897,7 +897,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1039,7 +1039,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1049,8 +1049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E2160"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C164" sqref="C164"/>
+    <sheetView tabSelected="1" topLeftCell="A1888" workbookViewId="0">
+      <selection activeCell="C1911" sqref="C1911"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24317,7 +24317,7 @@
         <v>2017</v>
       </c>
       <c r="C1905">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="1906" spans="1:3" x14ac:dyDescent="0.2">
@@ -24328,7 +24328,7 @@
         <v>2018</v>
       </c>
       <c r="C1906">
-        <v>100</v>
+        <v>60</v>
       </c>
     </row>
     <row r="1907" spans="1:3" x14ac:dyDescent="0.2">
@@ -24339,7 +24339,7 @@
         <v>2019</v>
       </c>
       <c r="C1907">
-        <v>100</v>
+        <v>60</v>
       </c>
     </row>
     <row r="1908" spans="1:3" x14ac:dyDescent="0.2">
@@ -24350,7 +24350,7 @@
         <v>2020</v>
       </c>
       <c r="C1908">
-        <v>100</v>
+        <v>60</v>
       </c>
     </row>
     <row r="1909" spans="1:3" x14ac:dyDescent="0.2">
@@ -24361,7 +24361,7 @@
         <v>2021</v>
       </c>
       <c r="C1909">
-        <v>100</v>
+        <v>60</v>
       </c>
     </row>
     <row r="1910" spans="1:3" x14ac:dyDescent="0.2">
@@ -24372,7 +24372,7 @@
         <v>2022</v>
       </c>
       <c r="C1910">
-        <v>100</v>
+        <v>60</v>
       </c>
     </row>
     <row r="1911" spans="1:3" x14ac:dyDescent="0.2">
@@ -24383,7 +24383,7 @@
         <v>2023</v>
       </c>
       <c r="C1911">
-        <v>100</v>
+        <v>60</v>
       </c>
     </row>
     <row r="1912" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>